<commit_message>
Atualização da Checklist para a fase de construção
</commit_message>
<xml_diff>
--- a/Wikipedia-Biologica-02/Desenvolvimento/4.Teste/WBio - Roteiro de Testes v1.0.xlsx
+++ b/Wikipedia-Biologica-02/Desenvolvimento/4.Teste/WBio - Roteiro de Testes v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\OneDrive\Área de Trabalho\Projetos IF\Wikipedia Biologica\WBio\Wikipedia-Biologica-02\Desenvolvimento\4.Teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC90E338-716B-4EDB-9821-576D9528AF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3741550C-18CB-4443-861F-2CCE2792E959}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="3255" windowWidth="21600" windowHeight="11385" tabRatio="913" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="913" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -29,19 +29,8 @@
     <definedName name="__xlfn_IFERROR">NA()</definedName>
     <definedName name="combo_SimNao">AUX!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -108,9 +97,6 @@
     <t>Qde. Ciclos</t>
   </si>
   <si>
-    <t>Dados da Matéria</t>
-  </si>
-  <si>
     <t>UC01</t>
   </si>
   <si>
@@ -265,6 +251,9 @@
   </si>
   <si>
     <t>Realização de login na plataforma</t>
+  </si>
+  <si>
+    <t>Dados dos Animais</t>
   </si>
 </sst>
 </file>
@@ -1450,7 +1439,7 @@
     <row r="2" spans="2:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24"/>
       <c r="C2" s="34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
@@ -1491,7 +1480,7 @@
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="25"/>
       <c r="C5" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="22">
         <v>1</v>
@@ -1504,7 +1493,7 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="25"/>
       <c r="C6" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="22">
         <v>2</v>
@@ -1517,7 +1506,7 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="25"/>
       <c r="C7" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="22">
         <v>1</v>
@@ -1530,7 +1519,7 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="25"/>
       <c r="C8" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="22">
         <v>1</v>
@@ -1543,7 +1532,7 @@
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="25"/>
       <c r="C9" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="22">
         <v>1</v>
@@ -1556,7 +1545,7 @@
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="25"/>
       <c r="C10" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="22">
         <v>3</v>
@@ -1569,7 +1558,7 @@
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="25"/>
       <c r="C11" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="22">
         <v>1</v>
@@ -1582,7 +1571,7 @@
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="25"/>
       <c r="C12" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="22">
         <v>1</v>
@@ -1723,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC6D9D-36DD-4683-8961-B6967A3741D3}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
@@ -1755,7 +1744,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1773,7 +1762,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1782,7 +1771,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1814,13 +1803,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="D9" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -2058,7 +2047,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -2076,7 +2065,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2085,7 +2074,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2117,13 +2106,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -2325,7 +2314,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -2343,7 +2332,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2352,7 +2341,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2384,13 +2373,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>47</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -2417,13 +2406,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -2565,9 +2554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576B397A-3A91-41DD-AA50-32F9E4528128}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2597,7 +2586,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -2615,7 +2604,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2654,11 +2643,11 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -2859,7 +2848,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -2877,7 +2866,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2916,13 +2905,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>54</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -3123,7 +3112,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -3178,11 +3167,11 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -3383,7 +3372,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -3401,7 +3390,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3440,13 +3429,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>61</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -3473,13 +3462,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -3506,13 +3495,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -3659,7 +3648,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -3677,7 +3666,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3686,7 +3675,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3718,13 +3707,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>68</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>

</xml_diff>